<commit_message>
update financial information (complete) - less fields
</commit_message>
<xml_diff>
--- a/Working Documents/financial_information.xlsx
+++ b/Working Documents/financial_information.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jeremy Chia\Documents\GitHub\NLP-SustainabilityReports-FinancialPerformance\Working Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E1E6CCA-8B3E-40DB-84DB-7F96686190D0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{90229CF2-EFF3-4575-8800-891FCCC35652}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1560" yWindow="1560" windowWidth="21600" windowHeight="11385" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2250" yWindow="2250" windowWidth="21600" windowHeight="11385" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="stagng" sheetId="3" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="273" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="266" uniqueCount="44">
   <si>
     <t>ASCENDAS REAL ESTATE INV TRUST</t>
   </si>
@@ -198,7 +198,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -214,6 +214,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="7" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -247,13 +253,15 @@
       <alignment horizontal="right"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="14" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="blp_column_header" xfId="1" xr:uid="{16DD0B64-D7F6-4404-B950-A201A9B92092}"/>
@@ -539,7 +547,7 @@
   <dimension ref="A2:H11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:H8"/>
+      <selection activeCell="C38" sqref="C38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -548,182 +556,182 @@
       <c r="A2" t="s">
         <v>32</v>
       </c>
-      <c r="B2" s="4" t="s">
-        <v>43</v>
+      <c r="B2" s="4">
+        <v>538.1</v>
       </c>
       <c r="C2" s="4">
-        <v>972.78930000000003</v>
+        <v>364.3</v>
       </c>
       <c r="D2" s="4">
-        <v>1393.6098</v>
+        <v>599.4</v>
       </c>
       <c r="E2" s="4">
-        <v>745.48429999999996</v>
+        <v>626.29999999999995</v>
       </c>
       <c r="F2" s="4">
-        <v>1004.6192</v>
+        <v>613.20000000000005</v>
       </c>
       <c r="G2" s="4">
-        <v>1009.0131</v>
+        <v>503.2</v>
       </c>
       <c r="H2" s="4">
-        <v>1056.9591</v>
+        <v>770.9</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>36</v>
       </c>
-      <c r="B3" s="4" t="s">
-        <v>43</v>
+      <c r="B3" s="4">
+        <v>538.1</v>
       </c>
       <c r="C3" s="4">
-        <v>972.78930000000003</v>
+        <v>364.3</v>
       </c>
       <c r="D3" s="4">
-        <v>1393.6098</v>
+        <v>599.4</v>
       </c>
       <c r="E3" s="4">
-        <v>745.48429999999996</v>
+        <v>626.29999999999995</v>
       </c>
       <c r="F3" s="4">
-        <v>1004.6192</v>
+        <v>613.20000000000005</v>
       </c>
       <c r="G3" s="4">
-        <v>1009.0131</v>
+        <v>503.2</v>
       </c>
       <c r="H3" s="4">
-        <v>1056.9591</v>
+        <v>770.9</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>39</v>
       </c>
-      <c r="B4" t="s">
-        <v>43</v>
+      <c r="B4">
+        <v>5637.1144000000004</v>
       </c>
       <c r="C4">
-        <v>1974.1277</v>
+        <v>5462.5892999999996</v>
       </c>
       <c r="D4">
-        <v>2277.7788999999998</v>
+        <v>6050.1750000000002</v>
       </c>
       <c r="E4">
-        <v>3182.3571999999999</v>
+        <v>6172.5517</v>
       </c>
       <c r="F4">
-        <v>3495.1356000000001</v>
+        <v>6034.6279000000004</v>
       </c>
       <c r="G4">
-        <v>3728.741</v>
+        <v>5896.6458000000002</v>
       </c>
       <c r="H4">
-        <v>3844.1844000000001</v>
+        <v>8173.8490000000002</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>38</v>
       </c>
-      <c r="B5" t="s">
-        <v>43</v>
+      <c r="B5">
+        <v>9009.6021999999994</v>
       </c>
       <c r="C5">
-        <v>7393.6691000000001</v>
+        <v>8596.5699000000004</v>
       </c>
       <c r="D5">
-        <v>7911.8116</v>
+        <v>8909.5683000000008</v>
       </c>
       <c r="E5">
-        <v>17679.2392</v>
+        <v>8899.3752999999997</v>
       </c>
       <c r="F5">
-        <v>18420.720799999999</v>
+        <v>8835.2932999999994</v>
       </c>
       <c r="G5">
-        <v>18727.8177</v>
+        <v>9091.2576000000008</v>
       </c>
       <c r="H5">
-        <v>19069.8102</v>
+        <v>10942.6672</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>40</v>
       </c>
-      <c r="B6" t="s">
-        <v>43</v>
+      <c r="B6">
+        <v>2389.5246000000002</v>
       </c>
       <c r="C6">
-        <v>1293.0799</v>
+        <v>2574.8809999999999</v>
       </c>
       <c r="D6">
-        <v>1941.7268999999999</v>
+        <v>2788.6936000000001</v>
       </c>
       <c r="E6">
-        <v>1584.6334999999999</v>
+        <v>2186.1010000000001</v>
       </c>
       <c r="F6">
-        <v>2206.3951999999999</v>
+        <v>1967.7927999999999</v>
       </c>
       <c r="G6">
-        <v>3920.4522000000002</v>
+        <v>1611.9154000000001</v>
       </c>
       <c r="H6">
-        <v>3851.3017</v>
+        <v>2501.5059000000001</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>37</v>
       </c>
-      <c r="B7" t="s">
-        <v>43</v>
+      <c r="B7">
+        <v>4125.6081000000004</v>
       </c>
       <c r="C7">
-        <v>2519.3220000000001</v>
+        <v>3759.9816999999998</v>
       </c>
       <c r="D7">
-        <v>2514.2831999999999</v>
+        <v>3462.5340999999999</v>
       </c>
       <c r="E7">
-        <v>11102.311900000001</v>
+        <v>2990.7501000000002</v>
       </c>
       <c r="F7">
-        <v>11625.490299999999</v>
+        <v>2645.7143999999998</v>
       </c>
       <c r="G7">
-        <v>10977.632299999999</v>
+        <v>2334.8552</v>
       </c>
       <c r="H7">
-        <v>10588.743399999999</v>
+        <v>3297.0095000000001</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>35</v>
       </c>
-      <c r="B8" t="s">
-        <v>43</v>
+      <c r="B8">
+        <v>4761.7593999999999</v>
       </c>
       <c r="C8">
-        <v>4730.8320000000003</v>
+        <v>4730.8581999999997</v>
       </c>
       <c r="D8">
-        <v>5245.4757</v>
+        <v>5317.2128000000002</v>
       </c>
       <c r="E8">
-        <v>5116.5834999999997</v>
+        <v>5766.5861999999997</v>
       </c>
       <c r="F8">
-        <v>5237.2237999999998</v>
+        <v>6004.4210000000003</v>
       </c>
       <c r="G8">
-        <v>6160.0870000000004</v>
+        <v>6547.0574999999999</v>
       </c>
       <c r="H8">
-        <v>6898.7240000000002</v>
+        <v>7616.3678</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
@@ -751,10 +759,10 @@
   <dimension ref="A1:M207"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="D173" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="1" topLeftCell="E146" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="D204" sqref="D204"/>
+      <selection pane="bottomRight" activeCell="F156" sqref="F156"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -958,10 +966,10 @@
         <f t="shared" si="0"/>
         <v>43830</v>
       </c>
-      <c r="D6" t="s">
+      <c r="D6" s="7" t="s">
         <v>43</v>
       </c>
-      <c r="E6" s="2" t="s">
+      <c r="E6" s="7" t="s">
         <v>43</v>
       </c>
       <c r="F6" s="2">
@@ -1288,25 +1296,25 @@
         <f t="shared" si="0"/>
         <v>42369</v>
       </c>
-      <c r="D16" t="s">
+      <c r="D16" s="6" t="s">
         <v>43</v>
       </c>
-      <c r="E16" t="s">
+      <c r="E16" s="6" t="s">
         <v>43</v>
       </c>
-      <c r="F16" s="2" t="s">
+      <c r="F16" s="6" t="s">
         <v>43</v>
       </c>
-      <c r="G16" s="2" t="s">
+      <c r="G16" s="6" t="s">
         <v>43</v>
       </c>
-      <c r="H16" s="2" t="s">
+      <c r="H16" s="6" t="s">
         <v>43</v>
       </c>
-      <c r="I16" s="2" t="s">
+      <c r="I16" s="6" t="s">
         <v>43</v>
       </c>
-      <c r="J16" s="2" t="s">
+      <c r="J16" s="6" t="s">
         <v>43</v>
       </c>
     </row>
@@ -1321,25 +1329,25 @@
         <f t="shared" si="0"/>
         <v>42735</v>
       </c>
-      <c r="D17" t="s">
+      <c r="D17" s="6" t="s">
         <v>43</v>
       </c>
-      <c r="E17" t="s">
+      <c r="E17" s="6" t="s">
         <v>43</v>
       </c>
-      <c r="F17" s="2" t="s">
+      <c r="F17" s="6" t="s">
         <v>43</v>
       </c>
-      <c r="G17" s="2" t="s">
+      <c r="G17" s="6" t="s">
         <v>43</v>
       </c>
-      <c r="H17" s="2" t="s">
+      <c r="H17" s="6" t="s">
         <v>43</v>
       </c>
-      <c r="I17" s="2" t="s">
+      <c r="I17" s="6" t="s">
         <v>43</v>
       </c>
-      <c r="J17" s="2" t="s">
+      <c r="J17" s="6" t="s">
         <v>43</v>
       </c>
     </row>
@@ -1354,25 +1362,25 @@
         <f t="shared" si="0"/>
         <v>43100</v>
       </c>
-      <c r="D18" t="s">
+      <c r="D18" s="6" t="s">
         <v>43</v>
       </c>
-      <c r="E18" t="s">
+      <c r="E18" s="6" t="s">
         <v>43</v>
       </c>
-      <c r="F18" s="2" t="s">
+      <c r="F18" s="6" t="s">
         <v>43</v>
       </c>
-      <c r="G18" s="2" t="s">
+      <c r="G18" s="6" t="s">
         <v>43</v>
       </c>
-      <c r="H18" s="2" t="s">
+      <c r="H18" s="6" t="s">
         <v>43</v>
       </c>
-      <c r="I18" s="2" t="s">
+      <c r="I18" s="6" t="s">
         <v>43</v>
       </c>
-      <c r="J18" s="2" t="s">
+      <c r="J18" s="6" t="s">
         <v>43</v>
       </c>
     </row>
@@ -1387,25 +1395,25 @@
         <f t="shared" si="0"/>
         <v>43465</v>
       </c>
-      <c r="D19" t="s">
+      <c r="D19" s="6" t="s">
         <v>43</v>
       </c>
-      <c r="E19" t="s">
+      <c r="E19" s="6" t="s">
         <v>43</v>
       </c>
-      <c r="F19" s="2" t="s">
+      <c r="F19" s="6" t="s">
         <v>43</v>
       </c>
-      <c r="G19" s="2" t="s">
+      <c r="G19" s="6" t="s">
         <v>43</v>
       </c>
-      <c r="H19" s="2" t="s">
+      <c r="H19" s="6" t="s">
         <v>43</v>
       </c>
-      <c r="I19" s="2" t="s">
+      <c r="I19" s="6" t="s">
         <v>43</v>
       </c>
-      <c r="J19" s="2" t="s">
+      <c r="J19" s="6" t="s">
         <v>43</v>
       </c>
     </row>
@@ -4858,7 +4866,10 @@
       <c r="B126">
         <v>2015</v>
       </c>
-      <c r="C126" s="3"/>
+      <c r="C126" s="5">
+        <f t="shared" ref="C126:C132" si="5">DATE(B126,3,31)</f>
+        <v>42094</v>
+      </c>
       <c r="D126">
         <v>195.69499999999999</v>
       </c>
@@ -4888,7 +4899,10 @@
       <c r="B127">
         <v>2016</v>
       </c>
-      <c r="C127" s="3"/>
+      <c r="C127" s="5">
+        <f t="shared" si="5"/>
+        <v>42460</v>
+      </c>
       <c r="D127">
         <v>220.59100000000001</v>
       </c>
@@ -4918,7 +4932,10 @@
       <c r="B128">
         <v>2017</v>
       </c>
-      <c r="C128" s="3"/>
+      <c r="C128" s="5">
+        <f t="shared" si="5"/>
+        <v>42825</v>
+      </c>
       <c r="D128">
         <v>257.935</v>
       </c>
@@ -4948,7 +4965,10 @@
       <c r="B129">
         <v>2018</v>
       </c>
-      <c r="C129" s="3"/>
+      <c r="C129" s="5">
+        <f t="shared" si="5"/>
+        <v>43190</v>
+      </c>
       <c r="D129">
         <v>261.46499999999997</v>
       </c>
@@ -4978,7 +4998,10 @@
       <c r="B130">
         <v>2019</v>
       </c>
-      <c r="C130" s="3"/>
+      <c r="C130" s="5">
+        <f t="shared" si="5"/>
+        <v>43555</v>
+      </c>
       <c r="D130">
         <v>248.40799999999999</v>
       </c>
@@ -5008,7 +5031,10 @@
       <c r="B131">
         <v>2020</v>
       </c>
-      <c r="C131" s="3"/>
+      <c r="C131" s="5">
+        <f t="shared" si="5"/>
+        <v>43921</v>
+      </c>
       <c r="D131">
         <v>168.36199999999999</v>
       </c>
@@ -5038,7 +5064,10 @@
       <c r="B132">
         <v>2021</v>
       </c>
-      <c r="C132" s="3"/>
+      <c r="C132" s="5">
+        <f t="shared" si="5"/>
+        <v>44286</v>
+      </c>
       <c r="D132">
         <v>-78.929000000000002</v>
       </c>
@@ -5068,7 +5097,10 @@
       <c r="B133">
         <v>2015</v>
       </c>
-      <c r="C133" s="3"/>
+      <c r="C133" s="1">
+        <f t="shared" ref="C133:C139" si="6">DATE(B133,12,31)</f>
+        <v>42369</v>
+      </c>
       <c r="D133">
         <v>548.85500000000002</v>
       </c>
@@ -5098,7 +5130,10 @@
       <c r="B134">
         <v>2016</v>
       </c>
-      <c r="C134" s="3"/>
+      <c r="C134" s="1">
+        <f t="shared" si="6"/>
+        <v>42735</v>
+      </c>
       <c r="D134">
         <v>394.88900000000001</v>
       </c>
@@ -5128,7 +5163,10 @@
       <c r="B135">
         <v>2017</v>
       </c>
-      <c r="C135" s="3"/>
+      <c r="C135" s="1">
+        <f t="shared" si="6"/>
+        <v>43100</v>
+      </c>
       <c r="D135">
         <v>383</v>
       </c>
@@ -5158,7 +5196,10 @@
       <c r="B136">
         <v>2018</v>
       </c>
-      <c r="C136" s="3"/>
+      <c r="C136" s="1">
+        <f t="shared" si="6"/>
+        <v>43465</v>
+      </c>
       <c r="D136">
         <v>347</v>
       </c>
@@ -5188,7 +5229,10 @@
       <c r="B137">
         <v>2019</v>
       </c>
-      <c r="C137" s="3"/>
+      <c r="C137" s="1">
+        <f t="shared" si="6"/>
+        <v>43830</v>
+      </c>
       <c r="D137">
         <v>247</v>
       </c>
@@ -5218,7 +5262,10 @@
       <c r="B138">
         <v>2020</v>
       </c>
-      <c r="C138" s="3"/>
+      <c r="C138" s="1">
+        <f t="shared" si="6"/>
+        <v>44196</v>
+      </c>
       <c r="D138">
         <v>-997</v>
       </c>
@@ -5248,7 +5295,10 @@
       <c r="B139">
         <v>2021</v>
       </c>
-      <c r="C139" s="3"/>
+      <c r="C139" s="1">
+        <f t="shared" si="6"/>
+        <v>44561</v>
+      </c>
       <c r="D139">
         <v>279</v>
       </c>
@@ -5278,7 +5328,10 @@
       <c r="B140">
         <v>2015</v>
       </c>
-      <c r="C140" s="3"/>
+      <c r="C140" s="5">
+        <f t="shared" ref="C140:C147" si="7">DATE(B140,3,31)</f>
+        <v>42094</v>
+      </c>
       <c r="D140">
         <v>367.9</v>
       </c>
@@ -5308,7 +5361,10 @@
       <c r="B141">
         <v>2016</v>
       </c>
-      <c r="C141" s="3"/>
+      <c r="C141" s="5">
+        <f t="shared" si="7"/>
+        <v>42460</v>
+      </c>
       <c r="D141">
         <v>804.4</v>
       </c>
@@ -5338,7 +5394,10 @@
       <c r="B142">
         <v>2017</v>
       </c>
-      <c r="C142" s="3"/>
+      <c r="C142" s="5">
+        <f t="shared" si="7"/>
+        <v>42825</v>
+      </c>
       <c r="D142">
         <v>360.4</v>
       </c>
@@ -5368,7 +5427,10 @@
       <c r="B143">
         <v>2018</v>
       </c>
-      <c r="C143" s="3"/>
+      <c r="C143" s="5">
+        <f t="shared" si="7"/>
+        <v>43190</v>
+      </c>
       <c r="D143">
         <v>1301.5999999999999</v>
       </c>
@@ -5398,7 +5460,10 @@
       <c r="B144">
         <v>2019</v>
       </c>
-      <c r="C144" s="3"/>
+      <c r="C144" s="5">
+        <f t="shared" si="7"/>
+        <v>43555</v>
+      </c>
       <c r="D144">
         <v>682.7</v>
       </c>
@@ -5428,7 +5493,10 @@
       <c r="B145">
         <v>2020</v>
       </c>
-      <c r="C145" s="3"/>
+      <c r="C145" s="5">
+        <f t="shared" si="7"/>
+        <v>43921</v>
+      </c>
       <c r="D145">
         <v>-212</v>
       </c>
@@ -5458,7 +5526,10 @@
       <c r="B146">
         <v>2021</v>
       </c>
-      <c r="C146" s="3"/>
+      <c r="C146" s="5">
+        <f t="shared" si="7"/>
+        <v>44286</v>
+      </c>
       <c r="D146">
         <v>-4270.7</v>
       </c>
@@ -5488,7 +5559,10 @@
       <c r="B147">
         <v>2015</v>
       </c>
-      <c r="C147" s="3"/>
+      <c r="C147" s="5">
+        <f>DATE(B147,6,30)</f>
+        <v>42185</v>
+      </c>
       <c r="D147">
         <v>348.61200000000002</v>
       </c>
@@ -5518,7 +5592,10 @@
       <c r="B148">
         <v>2016</v>
       </c>
-      <c r="C148" s="3"/>
+      <c r="C148" s="5">
+        <f t="shared" ref="C148:C153" si="8">DATE(B148,6,30)</f>
+        <v>42551</v>
+      </c>
       <c r="D148">
         <v>349.017</v>
       </c>
@@ -5548,7 +5625,10 @@
       <c r="B149">
         <v>2017</v>
       </c>
-      <c r="C149" s="3"/>
+      <c r="C149" s="5">
+        <f t="shared" si="8"/>
+        <v>42916</v>
+      </c>
       <c r="D149">
         <v>339.69200000000001</v>
       </c>
@@ -5578,7 +5658,10 @@
       <c r="B150">
         <v>2018</v>
       </c>
-      <c r="C150" s="3"/>
+      <c r="C150" s="5">
+        <f t="shared" si="8"/>
+        <v>43281</v>
+      </c>
       <c r="D150">
         <v>363.2</v>
       </c>
@@ -5608,7 +5691,10 @@
       <c r="B151">
         <v>2019</v>
       </c>
-      <c r="C151" s="3"/>
+      <c r="C151" s="5">
+        <f t="shared" si="8"/>
+        <v>43646</v>
+      </c>
       <c r="D151">
         <v>391.09800000000001</v>
       </c>
@@ -5638,7 +5724,10 @@
       <c r="B152">
         <v>2020</v>
       </c>
-      <c r="C152" s="3"/>
+      <c r="C152" s="5">
+        <f t="shared" si="8"/>
+        <v>44012</v>
+      </c>
       <c r="D152">
         <v>471.815</v>
       </c>
@@ -5668,7 +5757,10 @@
       <c r="B153">
         <v>2021</v>
       </c>
-      <c r="C153" s="3"/>
+      <c r="C153" s="5">
+        <f t="shared" si="8"/>
+        <v>44377</v>
+      </c>
       <c r="D153">
         <v>445.40600000000001</v>
       </c>
@@ -5698,7 +5790,10 @@
       <c r="B154">
         <v>2015</v>
       </c>
-      <c r="C154" s="3"/>
+      <c r="C154" s="1">
+        <f t="shared" ref="C154:C160" si="9">DATE(B154,12,31)</f>
+        <v>42369</v>
+      </c>
       <c r="D154">
         <v>529.03899999999999</v>
       </c>
@@ -5728,7 +5823,10 @@
       <c r="B155">
         <v>2016</v>
       </c>
-      <c r="C155" s="3"/>
+      <c r="C155" s="1">
+        <f t="shared" si="9"/>
+        <v>42735</v>
+      </c>
       <c r="D155">
         <v>484.51400000000001</v>
       </c>
@@ -5758,7 +5856,10 @@
       <c r="B156">
         <v>2017</v>
       </c>
-      <c r="C156" s="3"/>
+      <c r="C156" s="1">
+        <f t="shared" si="9"/>
+        <v>43100</v>
+      </c>
       <c r="D156">
         <v>502.63200000000001</v>
       </c>
@@ -5788,7 +5889,10 @@
       <c r="B157">
         <v>2018</v>
       </c>
-      <c r="C157" s="3"/>
+      <c r="C157" s="1">
+        <f t="shared" si="9"/>
+        <v>43465</v>
+      </c>
       <c r="D157">
         <v>494.24099999999999</v>
       </c>
@@ -5818,7 +5922,10 @@
       <c r="B158">
         <v>2019</v>
       </c>
-      <c r="C158" s="3"/>
+      <c r="C158" s="1">
+        <f t="shared" si="9"/>
+        <v>43830</v>
+      </c>
       <c r="D158">
         <v>577.94500000000005</v>
       </c>
@@ -5848,7 +5955,10 @@
       <c r="B159">
         <v>2020</v>
       </c>
-      <c r="C159" s="3"/>
+      <c r="C159" s="1">
+        <f t="shared" si="9"/>
+        <v>44196</v>
+      </c>
       <c r="D159">
         <v>521.84</v>
       </c>
@@ -5878,7 +5988,10 @@
       <c r="B160">
         <v>2021</v>
       </c>
-      <c r="C160" s="3"/>
+      <c r="C160" s="1">
+        <f t="shared" si="9"/>
+        <v>44561</v>
+      </c>
       <c r="D160">
         <v>570.54</v>
       </c>
@@ -5908,7 +6021,10 @@
       <c r="B161">
         <v>2015</v>
       </c>
-      <c r="C161" s="3"/>
+      <c r="C161" s="5">
+        <f t="shared" ref="C161:C167" si="10">DATE(B161,3,31)</f>
+        <v>42094</v>
+      </c>
       <c r="D161">
         <v>3781.5</v>
       </c>
@@ -5938,7 +6054,10 @@
       <c r="B162">
         <v>2016</v>
       </c>
-      <c r="C162" s="3"/>
+      <c r="C162" s="5">
+        <f t="shared" si="10"/>
+        <v>42460</v>
+      </c>
       <c r="D162">
         <v>3870.8</v>
       </c>
@@ -5968,7 +6087,10 @@
       <c r="B163">
         <v>2017</v>
       </c>
-      <c r="C163" s="3"/>
+      <c r="C163" s="5">
+        <f t="shared" si="10"/>
+        <v>42825</v>
+      </c>
       <c r="D163">
         <v>3852.7</v>
       </c>
@@ -5998,7 +6120,10 @@
       <c r="B164">
         <v>2018</v>
       </c>
-      <c r="C164" s="3"/>
+      <c r="C164" s="5">
+        <f t="shared" si="10"/>
+        <v>43190</v>
+      </c>
       <c r="D164">
         <v>5473</v>
       </c>
@@ -6028,7 +6153,10 @@
       <c r="B165">
         <v>2019</v>
       </c>
-      <c r="C165" s="3"/>
+      <c r="C165" s="5">
+        <f t="shared" si="10"/>
+        <v>43555</v>
+      </c>
       <c r="D165">
         <v>3094.5</v>
       </c>
@@ -6058,7 +6186,10 @@
       <c r="B166">
         <v>2020</v>
       </c>
-      <c r="C166" s="3"/>
+      <c r="C166" s="5">
+        <f t="shared" si="10"/>
+        <v>43921</v>
+      </c>
       <c r="D166">
         <v>1074.5999999999999</v>
       </c>
@@ -6088,7 +6219,10 @@
       <c r="B167">
         <v>2021</v>
       </c>
-      <c r="C167" s="3"/>
+      <c r="C167" s="5">
+        <f t="shared" si="10"/>
+        <v>44286</v>
+      </c>
       <c r="D167">
         <v>553.70000000000005</v>
       </c>
@@ -6118,26 +6252,29 @@
       <c r="B168">
         <v>2015</v>
       </c>
-      <c r="C168" s="3"/>
-      <c r="D168" t="s">
+      <c r="C168" s="5">
+        <f t="shared" ref="C168:C174" si="11">DATE(B168,9,30)</f>
+        <v>42277</v>
+      </c>
+      <c r="D168" s="6" t="s">
         <v>43</v>
       </c>
-      <c r="E168" s="2" t="s">
+      <c r="E168" s="6" t="s">
         <v>43</v>
       </c>
-      <c r="F168" s="2" t="s">
+      <c r="F168" s="6" t="s">
         <v>43</v>
       </c>
-      <c r="G168" s="2" t="s">
+      <c r="G168" s="6" t="s">
         <v>43</v>
       </c>
-      <c r="H168" s="2" t="s">
+      <c r="H168" s="6" t="s">
         <v>43</v>
       </c>
-      <c r="I168" s="2" t="s">
+      <c r="I168" s="6" t="s">
         <v>43</v>
       </c>
-      <c r="J168" s="2" t="s">
+      <c r="J168" s="6" t="s">
         <v>43</v>
       </c>
     </row>
@@ -6148,7 +6285,10 @@
       <c r="B169">
         <v>2016</v>
       </c>
-      <c r="C169" s="3"/>
+      <c r="C169" s="5">
+        <f t="shared" si="11"/>
+        <v>42643</v>
+      </c>
       <c r="D169">
         <v>972.78930000000003</v>
       </c>
@@ -6178,7 +6318,10 @@
       <c r="B170">
         <v>2017</v>
       </c>
-      <c r="C170" s="3"/>
+      <c r="C170" s="5">
+        <f t="shared" si="11"/>
+        <v>43008</v>
+      </c>
       <c r="D170">
         <v>1393.6098</v>
       </c>
@@ -6208,7 +6351,10 @@
       <c r="B171">
         <v>2018</v>
       </c>
-      <c r="C171" s="3"/>
+      <c r="C171" s="5">
+        <f t="shared" si="11"/>
+        <v>43373</v>
+      </c>
       <c r="D171">
         <v>745.48429999999996</v>
       </c>
@@ -6238,7 +6384,10 @@
       <c r="B172">
         <v>2019</v>
       </c>
-      <c r="C172" s="3"/>
+      <c r="C172" s="5">
+        <f t="shared" si="11"/>
+        <v>43738</v>
+      </c>
       <c r="D172">
         <v>1004.6192</v>
       </c>
@@ -6268,7 +6417,10 @@
       <c r="B173">
         <v>2020</v>
       </c>
-      <c r="C173" s="3"/>
+      <c r="C173" s="5">
+        <f t="shared" si="11"/>
+        <v>44104</v>
+      </c>
       <c r="D173">
         <v>1009.0131</v>
       </c>
@@ -6298,7 +6450,10 @@
       <c r="B174">
         <v>2021</v>
       </c>
-      <c r="C174" s="3"/>
+      <c r="C174" s="5">
+        <f t="shared" si="11"/>
+        <v>44469</v>
+      </c>
       <c r="D174">
         <v>1056.9591</v>
       </c>
@@ -6328,7 +6483,27 @@
       <c r="B175">
         <v>2015</v>
       </c>
-      <c r="C175" s="3"/>
+      <c r="C175" s="1">
+        <f t="shared" ref="C175:C207" si="12">DATE(B175,12,31)</f>
+        <v>42369</v>
+      </c>
+      <c r="D175">
+        <v>3208.8989999999999</v>
+      </c>
+      <c r="E175" s="2">
+        <v>3208.8989999999999</v>
+      </c>
+      <c r="F175" s="3"/>
+      <c r="G175" s="2">
+        <v>316011.20500000002</v>
+      </c>
+      <c r="H175" s="3"/>
+      <c r="I175" s="2">
+        <v>285087.43199999997</v>
+      </c>
+      <c r="J175" s="2">
+        <v>30768.405999999999</v>
+      </c>
     </row>
     <row r="176" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A176" t="s">
@@ -6337,286 +6512,1030 @@
       <c r="B176">
         <v>2016</v>
       </c>
-      <c r="C176" s="3"/>
-    </row>
-    <row r="177" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C176" s="1">
+        <f t="shared" si="12"/>
+        <v>42735</v>
+      </c>
+      <c r="D176">
+        <v>3096.2890000000002</v>
+      </c>
+      <c r="E176" s="2">
+        <v>3096.2890000000002</v>
+      </c>
+      <c r="F176" s="3"/>
+      <c r="G176" s="2">
+        <v>340027.63299999997</v>
+      </c>
+      <c r="H176" s="3"/>
+      <c r="I176" s="2">
+        <v>306985.84499999997</v>
+      </c>
+      <c r="J176" s="2">
+        <v>32873.188999999998</v>
+      </c>
+    </row>
+    <row r="177" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A177" t="s">
         <v>25</v>
       </c>
       <c r="B177">
         <v>2017</v>
       </c>
-      <c r="C177" s="3"/>
-    </row>
-    <row r="178" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C177" s="1">
+        <f t="shared" si="12"/>
+        <v>43100</v>
+      </c>
+      <c r="D177">
+        <v>3390.2910000000002</v>
+      </c>
+      <c r="E177" s="2">
+        <v>3390.2910000000002</v>
+      </c>
+      <c r="F177" s="3"/>
+      <c r="G177" s="2">
+        <v>358592.36300000001</v>
+      </c>
+      <c r="H177" s="3"/>
+      <c r="I177" s="2">
+        <v>321555.76799999998</v>
+      </c>
+      <c r="J177" s="2">
+        <v>36849.934000000001</v>
+      </c>
+    </row>
+    <row r="178" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A178" t="s">
         <v>25</v>
       </c>
       <c r="B178">
         <v>2018</v>
       </c>
-      <c r="C178" s="3"/>
-    </row>
-    <row r="179" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C178" s="1">
+        <f t="shared" si="12"/>
+        <v>43465</v>
+      </c>
+      <c r="D178">
+        <v>4008.0010000000002</v>
+      </c>
+      <c r="E178" s="2">
+        <v>4008.0010000000002</v>
+      </c>
+      <c r="F178" s="3"/>
+      <c r="G178" s="2">
+        <v>388092.35499999998</v>
+      </c>
+      <c r="H178" s="3"/>
+      <c r="I178" s="2">
+        <v>350279.56300000002</v>
+      </c>
+      <c r="J178" s="2">
+        <v>37623.095999999998</v>
+      </c>
+    </row>
+    <row r="179" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A179" t="s">
         <v>25</v>
       </c>
       <c r="B179">
         <v>2019</v>
       </c>
-      <c r="C179" s="3"/>
-    </row>
-    <row r="180" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C179" s="1">
+        <f t="shared" si="12"/>
+        <v>43830</v>
+      </c>
+      <c r="D179">
+        <v>4343.3459999999995</v>
+      </c>
+      <c r="E179" s="2">
+        <v>4343.3459999999995</v>
+      </c>
+      <c r="F179" s="3"/>
+      <c r="G179" s="2">
+        <v>404408.58</v>
+      </c>
+      <c r="H179" s="3"/>
+      <c r="I179" s="2">
+        <v>364544.65500000003</v>
+      </c>
+      <c r="J179" s="2">
+        <v>39636.51</v>
+      </c>
+    </row>
+    <row r="180" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A180" t="s">
         <v>25</v>
       </c>
       <c r="B180">
         <v>2020</v>
       </c>
-      <c r="C180" s="3"/>
-    </row>
-    <row r="181" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C180" s="1">
+        <f t="shared" si="12"/>
+        <v>44196</v>
+      </c>
+      <c r="D180">
+        <v>2915</v>
+      </c>
+      <c r="E180" s="2">
+        <v>2915</v>
+      </c>
+      <c r="F180" s="3"/>
+      <c r="G180" s="2">
+        <v>431814</v>
+      </c>
+      <c r="H180" s="3"/>
+      <c r="I180" s="2">
+        <v>390683</v>
+      </c>
+      <c r="J180" s="2">
+        <v>40901</v>
+      </c>
+    </row>
+    <row r="181" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A181" t="s">
         <v>25</v>
       </c>
       <c r="B181">
         <v>2021</v>
       </c>
-      <c r="C181" s="3"/>
-    </row>
-    <row r="182" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C181" s="1">
+        <f t="shared" si="12"/>
+        <v>44561</v>
+      </c>
+      <c r="D181">
+        <v>4075</v>
+      </c>
+      <c r="E181" s="2">
+        <v>4075</v>
+      </c>
+      <c r="F181" s="3"/>
+      <c r="G181" s="2">
+        <v>459323</v>
+      </c>
+      <c r="H181" s="3"/>
+      <c r="I181" s="2">
+        <v>416462</v>
+      </c>
+      <c r="J181" s="2">
+        <v>42633</v>
+      </c>
+    </row>
+    <row r="182" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A182" t="s">
         <v>26</v>
       </c>
       <c r="B182">
         <v>2015</v>
       </c>
-      <c r="C182" s="3"/>
-    </row>
-    <row r="183" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C182" s="1">
+        <f t="shared" si="12"/>
+        <v>42369</v>
+      </c>
+      <c r="D182">
+        <v>391.38900000000001</v>
+      </c>
+      <c r="E182" s="2">
+        <v>391.38900000000001</v>
+      </c>
+      <c r="F182" s="2">
+        <v>1975.6110000000001</v>
+      </c>
+      <c r="G182" s="2">
+        <v>11501.281000000001</v>
+      </c>
+      <c r="H182" s="2">
+        <v>803.71500000000003</v>
+      </c>
+      <c r="I182" s="2">
+        <v>3100.165</v>
+      </c>
+      <c r="J182" s="2">
+        <v>7894.1750000000002</v>
+      </c>
+    </row>
+    <row r="183" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A183" t="s">
         <v>26</v>
       </c>
       <c r="B183">
         <v>2016</v>
       </c>
-      <c r="C183" s="3"/>
-    </row>
-    <row r="184" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C183" s="1">
+        <f t="shared" si="12"/>
+        <v>42735</v>
+      </c>
+      <c r="D183">
+        <v>287.04000000000002</v>
+      </c>
+      <c r="E183" s="2">
+        <v>287.04000000000002</v>
+      </c>
+      <c r="F183" s="2">
+        <v>1593.13</v>
+      </c>
+      <c r="G183" s="2">
+        <v>11558.14</v>
+      </c>
+      <c r="H183" s="2">
+        <v>982.49900000000002</v>
+      </c>
+      <c r="I183" s="2">
+        <v>2922.7759999999998</v>
+      </c>
+      <c r="J183" s="2">
+        <v>8127.1540000000005</v>
+      </c>
+    </row>
+    <row r="184" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A184" t="s">
         <v>26</v>
       </c>
       <c r="B184">
         <v>2017</v>
       </c>
-      <c r="C184" s="3"/>
-    </row>
-    <row r="185" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C184" s="1">
+        <f t="shared" si="12"/>
+        <v>43100</v>
+      </c>
+      <c r="D184">
+        <v>880.23900000000003</v>
+      </c>
+      <c r="E184" s="2">
+        <v>880.23900000000003</v>
+      </c>
+      <c r="F184" s="2">
+        <v>4164.3959999999997</v>
+      </c>
+      <c r="G184" s="2">
+        <v>19632.501</v>
+      </c>
+      <c r="H184" s="2">
+        <v>2009.971</v>
+      </c>
+      <c r="I184" s="2">
+        <v>5478.6940000000004</v>
+      </c>
+      <c r="J184" s="2">
+        <v>9451.1329999999998</v>
+      </c>
+    </row>
+    <row r="185" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A185" t="s">
         <v>26</v>
       </c>
       <c r="B185">
         <v>2018</v>
       </c>
-      <c r="C185" s="3"/>
-    </row>
-    <row r="186" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C185" s="1">
+        <f t="shared" si="12"/>
+        <v>43465</v>
+      </c>
+      <c r="D185">
+        <v>418.30399999999997</v>
+      </c>
+      <c r="E185" s="2">
+        <v>418.30399999999997</v>
+      </c>
+      <c r="F185" s="2">
+        <v>4936.6750000000002</v>
+      </c>
+      <c r="G185" s="2">
+        <v>20620.359</v>
+      </c>
+      <c r="H185" s="2">
+        <v>2753.3310000000001</v>
+      </c>
+      <c r="I185" s="2">
+        <v>6186.7110000000002</v>
+      </c>
+      <c r="J185" s="2">
+        <v>9621.0509999999995</v>
+      </c>
+    </row>
+    <row r="186" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A186" t="s">
         <v>26</v>
       </c>
       <c r="B186">
         <v>2019</v>
       </c>
-      <c r="C186" s="3"/>
-    </row>
-    <row r="187" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C186" s="1">
+        <f t="shared" si="12"/>
+        <v>43830</v>
+      </c>
+      <c r="D186">
+        <v>478.81700000000001</v>
+      </c>
+      <c r="E186" s="2">
+        <v>478.81700000000001</v>
+      </c>
+      <c r="F186" s="2">
+        <v>4481.4769999999999</v>
+      </c>
+      <c r="G186" s="2">
+        <v>20653.774000000001</v>
+      </c>
+      <c r="H186" s="2">
+        <v>2510.9639999999999</v>
+      </c>
+      <c r="I186" s="2">
+        <v>6319.4849999999997</v>
+      </c>
+      <c r="J186" s="2">
+        <v>10047.48</v>
+      </c>
+    </row>
+    <row r="187" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A187" t="s">
         <v>26</v>
       </c>
       <c r="B187">
         <v>2020</v>
       </c>
-      <c r="C187" s="3"/>
-    </row>
-    <row r="188" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C187" s="1">
+        <f t="shared" si="12"/>
+        <v>44196</v>
+      </c>
+      <c r="D187">
+        <v>13.141</v>
+      </c>
+      <c r="E187" s="2">
+        <v>13.141</v>
+      </c>
+      <c r="F187" s="2">
+        <v>4506.3969999999999</v>
+      </c>
+      <c r="G187" s="2">
+        <v>20373.493999999999</v>
+      </c>
+      <c r="H187" s="2">
+        <v>2336.77</v>
+      </c>
+      <c r="I187" s="2">
+        <v>6272.3459999999995</v>
+      </c>
+      <c r="J187" s="2">
+        <v>9788.1409999999996</v>
+      </c>
+    </row>
+    <row r="188" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A188" t="s">
         <v>26</v>
       </c>
       <c r="B188">
         <v>2021</v>
       </c>
-      <c r="C188" s="3"/>
-    </row>
-    <row r="189" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C188" s="1">
+        <f t="shared" si="12"/>
+        <v>44561</v>
+      </c>
+      <c r="D188">
+        <v>307.411</v>
+      </c>
+      <c r="E188" s="2">
+        <v>307.411</v>
+      </c>
+      <c r="F188" s="2">
+        <v>4996.5630000000001</v>
+      </c>
+      <c r="G188" s="2">
+        <v>21274.971000000001</v>
+      </c>
+      <c r="H188" s="2">
+        <v>2479.3440000000001</v>
+      </c>
+      <c r="I188" s="2">
+        <v>6658.8959999999997</v>
+      </c>
+      <c r="J188" s="2">
+        <v>10168.323</v>
+      </c>
+    </row>
+    <row r="189" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A189" t="s">
         <v>27</v>
       </c>
       <c r="B189">
         <v>2017</v>
       </c>
-      <c r="C189" s="3"/>
-    </row>
-    <row r="190" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C189" s="1">
+        <f t="shared" si="12"/>
+        <v>43100</v>
+      </c>
+      <c r="D189">
+        <v>454.95699999999999</v>
+      </c>
+      <c r="E189" s="2">
+        <v>454.95699999999999</v>
+      </c>
+      <c r="F189" s="2">
+        <v>2276.1559999999999</v>
+      </c>
+      <c r="G189" s="2">
+        <v>3144.2049999999999</v>
+      </c>
+      <c r="H189" s="2">
+        <v>974.423</v>
+      </c>
+      <c r="I189" s="2">
+        <v>976.14099999999996</v>
+      </c>
+      <c r="J189" s="2">
+        <v>2165.75</v>
+      </c>
+    </row>
+    <row r="190" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A190" t="s">
         <v>27</v>
       </c>
       <c r="B190">
         <v>2018</v>
       </c>
-      <c r="C190" s="3"/>
-    </row>
-    <row r="191" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C190" s="1">
+        <f t="shared" si="12"/>
+        <v>43465</v>
+      </c>
+      <c r="D190">
+        <v>262.99400000000003</v>
+      </c>
+      <c r="E190" s="2">
+        <v>262.99400000000003</v>
+      </c>
+      <c r="F190" s="2">
+        <v>2306.1559999999999</v>
+      </c>
+      <c r="G190" s="2">
+        <v>3204.5970000000002</v>
+      </c>
+      <c r="H190" s="2">
+        <v>850.44</v>
+      </c>
+      <c r="I190" s="2">
+        <v>852.49800000000005</v>
+      </c>
+      <c r="J190" s="2">
+        <v>2349.866</v>
+      </c>
+    </row>
+    <row r="191" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A191" t="s">
         <v>27</v>
       </c>
       <c r="B191">
         <v>2019</v>
       </c>
-      <c r="C191" s="3"/>
-    </row>
-    <row r="192" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C191" s="1">
+        <f t="shared" si="12"/>
+        <v>43830</v>
+      </c>
+      <c r="D191">
+        <v>241.18</v>
+      </c>
+      <c r="E191" s="2">
+        <v>241.18</v>
+      </c>
+      <c r="F191" s="2">
+        <v>2345.3359999999998</v>
+      </c>
+      <c r="G191" s="2">
+        <v>3274.2449999999999</v>
+      </c>
+      <c r="H191" s="2">
+        <v>755.29399999999998</v>
+      </c>
+      <c r="I191" s="2">
+        <v>775.65200000000004</v>
+      </c>
+      <c r="J191" s="2">
+        <v>2496.1979999999999</v>
+      </c>
+    </row>
+    <row r="192" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A192" t="s">
         <v>27</v>
       </c>
       <c r="B192">
         <v>2020</v>
       </c>
-      <c r="C192" s="3"/>
-    </row>
-    <row r="193" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C192" s="1">
+        <f t="shared" si="12"/>
+        <v>44196</v>
+      </c>
+      <c r="D192">
+        <v>461.13900000000001</v>
+      </c>
+      <c r="E192" s="2">
+        <v>461.13900000000001</v>
+      </c>
+      <c r="F192" s="2">
+        <v>2323.33</v>
+      </c>
+      <c r="G192" s="2">
+        <v>3239.567</v>
+      </c>
+      <c r="H192" s="2">
+        <v>636.22799999999995</v>
+      </c>
+      <c r="I192" s="2">
+        <v>650.43799999999999</v>
+      </c>
+      <c r="J192" s="2">
+        <v>2586.4499999999998</v>
+      </c>
+    </row>
+    <row r="193" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A193" t="s">
         <v>27</v>
       </c>
       <c r="B193">
         <v>2021</v>
       </c>
-      <c r="C193" s="3"/>
-    </row>
-    <row r="194" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C193" s="1">
+        <f t="shared" si="12"/>
+        <v>44561</v>
+      </c>
+      <c r="D193">
+        <v>108.08799999999999</v>
+      </c>
+      <c r="E193" s="2">
+        <v>108.08799999999999</v>
+      </c>
+      <c r="F193" s="2">
+        <v>2737.5210000000002</v>
+      </c>
+      <c r="G193" s="2">
+        <v>3635.261</v>
+      </c>
+      <c r="H193" s="2">
+        <v>907.49900000000002</v>
+      </c>
+      <c r="I193" s="2">
+        <v>915.81100000000004</v>
+      </c>
+      <c r="J193" s="2">
+        <v>2716.3519999999999</v>
+      </c>
+    </row>
+    <row r="194" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A194" t="s">
         <v>28</v>
       </c>
       <c r="B194">
         <v>2015</v>
       </c>
-      <c r="C194" s="3"/>
-    </row>
-    <row r="195" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C194" s="1">
+        <f t="shared" si="12"/>
+        <v>42369</v>
+      </c>
+      <c r="D194">
+        <v>1406.405</v>
+      </c>
+      <c r="E194" s="2">
+        <v>1406.405</v>
+      </c>
+      <c r="F194" s="2">
+        <v>26735.840400000001</v>
+      </c>
+      <c r="G194" s="2">
+        <v>52327.836000000003</v>
+      </c>
+      <c r="H194" s="2">
+        <v>20818.283100000001</v>
+      </c>
+      <c r="I194" s="2">
+        <v>30644.6826</v>
+      </c>
+      <c r="J194" s="2">
+        <v>20397.934399999998</v>
+      </c>
+    </row>
+    <row r="195" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A195" t="s">
         <v>28</v>
       </c>
       <c r="B195">
         <v>2016</v>
       </c>
-      <c r="C195" s="3"/>
-    </row>
-    <row r="196" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C195" s="1">
+        <f t="shared" si="12"/>
+        <v>42735</v>
+      </c>
+      <c r="D195">
+        <v>1342.454</v>
+      </c>
+      <c r="E195" s="2">
+        <v>1342.454</v>
+      </c>
+      <c r="F195" s="2">
+        <v>28119.457900000001</v>
+      </c>
+      <c r="G195" s="2">
+        <v>53578.513899999998</v>
+      </c>
+      <c r="H195" s="2">
+        <v>24195.047600000002</v>
+      </c>
+      <c r="I195" s="2">
+        <v>31328.2274</v>
+      </c>
+      <c r="J195" s="2">
+        <v>20883.8838</v>
+      </c>
+    </row>
+    <row r="196" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A196" t="s">
         <v>28</v>
       </c>
       <c r="B196">
         <v>2017</v>
       </c>
-      <c r="C196" s="3"/>
-    </row>
-    <row r="197" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C196" s="1">
+        <f t="shared" si="12"/>
+        <v>43100</v>
+      </c>
+      <c r="D196">
+        <v>1650.8412000000001</v>
+      </c>
+      <c r="E196" s="2">
+        <v>1650.8412000000001</v>
+      </c>
+      <c r="F196" s="2">
+        <v>30179.621999999999</v>
+      </c>
+      <c r="G196" s="2">
+        <v>54710.477099999996</v>
+      </c>
+      <c r="H196" s="2">
+        <v>26313.816599999998</v>
+      </c>
+      <c r="I196" s="2">
+        <v>32008.1937</v>
+      </c>
+      <c r="J196" s="2">
+        <v>21336.937099999999</v>
+      </c>
+    </row>
+    <row r="197" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A197" t="s">
         <v>28</v>
       </c>
       <c r="B197">
         <v>2018</v>
       </c>
-      <c r="C197" s="3"/>
-    </row>
-    <row r="198" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C197" s="1">
+        <f t="shared" si="12"/>
+        <v>43465</v>
+      </c>
+      <c r="D197">
+        <v>1517.72</v>
+      </c>
+      <c r="E197" s="2">
+        <v>1517.72</v>
+      </c>
+      <c r="F197" s="2">
+        <v>35833.820699999997</v>
+      </c>
+      <c r="G197" s="2">
+        <v>62306.728999999999</v>
+      </c>
+      <c r="H197" s="2">
+        <v>31131.327499999999</v>
+      </c>
+      <c r="I197" s="2">
+        <v>39442.3822</v>
+      </c>
+      <c r="J197" s="2">
+        <v>21870.3927</v>
+      </c>
+    </row>
+    <row r="198" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A198" t="s">
         <v>28</v>
       </c>
       <c r="B198">
         <v>2019</v>
       </c>
-      <c r="C198" s="3"/>
-    </row>
-    <row r="199" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C198" s="1">
+        <f t="shared" si="12"/>
+        <v>43830</v>
+      </c>
+      <c r="D198">
+        <v>1764.3389</v>
+      </c>
+      <c r="E198" s="2">
+        <v>1764.3389</v>
+      </c>
+      <c r="F198" s="2">
+        <v>34399.844400000002</v>
+      </c>
+      <c r="G198" s="2">
+        <v>63256.900600000001</v>
+      </c>
+      <c r="H198" s="2">
+        <v>30910.885699999999</v>
+      </c>
+      <c r="I198" s="2">
+        <v>39220.672400000003</v>
+      </c>
+      <c r="J198" s="2">
+        <v>22538.869600000002</v>
+      </c>
+    </row>
+    <row r="199" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A199" t="s">
         <v>28</v>
       </c>
       <c r="B199">
         <v>2020</v>
       </c>
-      <c r="C199" s="3"/>
-    </row>
-    <row r="200" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C199" s="1">
+        <f t="shared" si="12"/>
+        <v>44196</v>
+      </c>
+      <c r="D199">
+        <v>2115.8251</v>
+      </c>
+      <c r="E199" s="2">
+        <v>2115.8251</v>
+      </c>
+      <c r="F199" s="2">
+        <v>36895.413</v>
+      </c>
+      <c r="G199" s="2">
+        <v>67412.694300000003</v>
+      </c>
+      <c r="H199" s="2">
+        <v>30169.449000000001</v>
+      </c>
+      <c r="I199" s="2">
+        <v>39158.930699999997</v>
+      </c>
+      <c r="J199" s="2">
+        <v>24949.255700000002</v>
+      </c>
+    </row>
+    <row r="200" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A200" t="s">
         <v>28</v>
       </c>
       <c r="B200">
         <v>2021</v>
       </c>
-      <c r="C200" s="3"/>
-    </row>
-    <row r="201" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C200" s="1">
+        <f t="shared" si="12"/>
+        <v>44561</v>
+      </c>
+      <c r="D200">
+        <v>2540.3339999999998</v>
+      </c>
+      <c r="E200" s="2">
+        <v>2540.3339999999998</v>
+      </c>
+      <c r="F200" s="2">
+        <v>42873.891300000003</v>
+      </c>
+      <c r="G200" s="2">
+        <v>79128.977799999993</v>
+      </c>
+      <c r="H200" s="2">
+        <v>38262.718099999998</v>
+      </c>
+      <c r="I200" s="2">
+        <v>48670.079299999998</v>
+      </c>
+      <c r="J200" s="2">
+        <v>26849.414000000001</v>
+      </c>
+    </row>
+    <row r="201" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A201" t="s">
         <v>29</v>
       </c>
       <c r="B201">
         <v>2015</v>
       </c>
-      <c r="C201" s="3"/>
-    </row>
-    <row r="202" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C201" s="1">
+        <f t="shared" si="12"/>
+        <v>42369</v>
+      </c>
+      <c r="D201">
+        <v>538.1</v>
+      </c>
+      <c r="E201" s="2">
+        <v>538.1</v>
+      </c>
+      <c r="F201" s="2">
+        <v>5637.1144000000004</v>
+      </c>
+      <c r="G201" s="2">
+        <v>9009.6021999999994</v>
+      </c>
+      <c r="H201" s="2">
+        <v>2389.5246000000002</v>
+      </c>
+      <c r="I201" s="2">
+        <v>4125.6081000000004</v>
+      </c>
+      <c r="J201" s="2">
+        <v>4761.7593999999999</v>
+      </c>
+    </row>
+    <row r="202" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A202" t="s">
         <v>29</v>
       </c>
       <c r="B202">
         <v>2016</v>
       </c>
-      <c r="C202" s="3"/>
-    </row>
-    <row r="203" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C202" s="1">
+        <f t="shared" si="12"/>
+        <v>42735</v>
+      </c>
+      <c r="D202">
+        <v>364.3</v>
+      </c>
+      <c r="E202" s="2">
+        <v>364.3</v>
+      </c>
+      <c r="F202" s="2">
+        <v>5462.5892999999996</v>
+      </c>
+      <c r="G202" s="2">
+        <v>8596.5699000000004</v>
+      </c>
+      <c r="H202" s="2">
+        <v>2574.8809999999999</v>
+      </c>
+      <c r="I202" s="2">
+        <v>3759.9816999999998</v>
+      </c>
+      <c r="J202" s="2">
+        <v>4730.8581999999997</v>
+      </c>
+    </row>
+    <row r="203" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A203" t="s">
         <v>29</v>
       </c>
       <c r="B203">
         <v>2017</v>
       </c>
-      <c r="C203" s="3"/>
-    </row>
-    <row r="204" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C203" s="1">
+        <f t="shared" si="12"/>
+        <v>43100</v>
+      </c>
+      <c r="D203">
+        <v>599.4</v>
+      </c>
+      <c r="E203" s="2">
+        <v>599.4</v>
+      </c>
+      <c r="F203" s="2">
+        <v>6050.1750000000002</v>
+      </c>
+      <c r="G203" s="2">
+        <v>8909.5683000000008</v>
+      </c>
+      <c r="H203" s="2">
+        <v>2788.6936000000001</v>
+      </c>
+      <c r="I203" s="2">
+        <v>3462.5340999999999</v>
+      </c>
+      <c r="J203" s="2">
+        <v>5317.2128000000002</v>
+      </c>
+    </row>
+    <row r="204" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A204" t="s">
         <v>29</v>
       </c>
       <c r="B204">
         <v>2018</v>
       </c>
-      <c r="C204" s="3"/>
-    </row>
-    <row r="205" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C204" s="1">
+        <f t="shared" si="12"/>
+        <v>43465</v>
+      </c>
+      <c r="D204">
+        <v>626.29999999999995</v>
+      </c>
+      <c r="E204" s="2">
+        <v>626.29999999999995</v>
+      </c>
+      <c r="F204" s="2">
+        <v>6172.5517</v>
+      </c>
+      <c r="G204" s="2">
+        <v>8899.3752999999997</v>
+      </c>
+      <c r="H204" s="2">
+        <v>2186.1010000000001</v>
+      </c>
+      <c r="I204" s="2">
+        <v>2990.7501000000002</v>
+      </c>
+      <c r="J204" s="2">
+        <v>5766.5861999999997</v>
+      </c>
+    </row>
+    <row r="205" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A205" t="s">
         <v>29</v>
       </c>
       <c r="B205">
         <v>2019</v>
       </c>
-      <c r="C205" s="3"/>
-    </row>
-    <row r="206" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C205" s="1">
+        <f t="shared" si="12"/>
+        <v>43830</v>
+      </c>
+      <c r="D205">
+        <v>613.20000000000005</v>
+      </c>
+      <c r="E205" s="2">
+        <v>613.20000000000005</v>
+      </c>
+      <c r="F205" s="2">
+        <v>6034.6279000000004</v>
+      </c>
+      <c r="G205" s="2">
+        <v>8835.2932999999994</v>
+      </c>
+      <c r="H205" s="2">
+        <v>1967.7927999999999</v>
+      </c>
+      <c r="I205" s="2">
+        <v>2645.7143999999998</v>
+      </c>
+      <c r="J205" s="2">
+        <v>6004.4210000000003</v>
+      </c>
+    </row>
+    <row r="206" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A206" t="s">
         <v>29</v>
       </c>
       <c r="B206">
         <v>2020</v>
       </c>
-      <c r="C206" s="3"/>
-    </row>
-    <row r="207" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C206" s="1">
+        <f t="shared" si="12"/>
+        <v>44196</v>
+      </c>
+      <c r="D206">
+        <v>503.2</v>
+      </c>
+      <c r="E206" s="2">
+        <v>503.2</v>
+      </c>
+      <c r="F206" s="2">
+        <v>5896.6458000000002</v>
+      </c>
+      <c r="G206" s="2">
+        <v>9091.2576000000008</v>
+      </c>
+      <c r="H206" s="2">
+        <v>1611.9154000000001</v>
+      </c>
+      <c r="I206" s="2">
+        <v>2334.8552</v>
+      </c>
+      <c r="J206" s="2">
+        <v>6547.0574999999999</v>
+      </c>
+    </row>
+    <row r="207" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A207" t="s">
         <v>29</v>
       </c>
       <c r="B207">
         <v>2021</v>
       </c>
-      <c r="C207" s="3"/>
+      <c r="C207" s="1">
+        <f t="shared" si="12"/>
+        <v>44561</v>
+      </c>
+      <c r="D207">
+        <v>770.9</v>
+      </c>
+      <c r="E207" s="2">
+        <v>770.9</v>
+      </c>
+      <c r="F207" s="2">
+        <v>8173.8490000000002</v>
+      </c>
+      <c r="G207" s="2">
+        <v>10942.6672</v>
+      </c>
+      <c r="H207" s="2">
+        <v>2501.5059000000001</v>
+      </c>
+      <c r="I207" s="2">
+        <v>3297.0095000000001</v>
+      </c>
+      <c r="J207" s="2">
+        <v>7616.3678</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>